<commit_message>
feil lsit for 12 uF opdater til rikgit
</commit_message>
<xml_diff>
--- a/Hardware/Altium/Handle og komponent liste til pcb.xlsx
+++ b/Hardware/Altium/Handle og komponent liste til pcb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Documents\GitHub\Bachelor-Nordic_Semi\Hardware\Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="370" documentId="8_{32C0A267-AC62-48FA-B9E9-63A7E08ECCE9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{B17F2090-28DC-4687-9B5F-2D08A32FEA7A}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{32C0A267-AC62-48FA-B9E9-63A7E08ECCE9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{4A5F7AA9-0512-4685-846F-156071B62C21}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8120" windowHeight="12040" xr2:uid="{1A450696-9875-48AE-A124-9F1ED327ADC9}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>diode</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GQM1875C2E560JB12D/490-7175-1-ND/3900438</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=260184054&amp;uq=636613683072925453</t>
   </si>
   <si>
@@ -448,6 +445,9 @@
   </si>
   <si>
     <t>28,47USD + nrf52 og pcb</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-corporation/C3225X5R0J686M200AC/445-3954-1-ND/1944451</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2614B9A-97C1-446F-A337-94A97A3D3E09}">
   <dimension ref="A4:AC77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S74" sqref="S74"/>
+    <sheetView tabSelected="1" topLeftCell="G15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,7 +1240,7 @@
         <v>43</v>
       </c>
       <c r="AC19" s="38" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.35">
@@ -1416,7 +1416,7 @@
         <v>46</v>
       </c>
       <c r="AC25" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.35">
@@ -2596,10 +2596,10 @@
         <v>120</v>
       </c>
       <c r="Y72" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z72" t="s">
         <v>139</v>
-      </c>
-      <c r="Z72" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="73" spans="2:29" x14ac:dyDescent="0.35">
@@ -2723,8 +2723,9 @@
     <hyperlink ref="AC57" r:id="rId31" xr:uid="{0674174B-488E-4522-B899-05070EDEC14D}"/>
     <hyperlink ref="AC58" r:id="rId32" xr:uid="{E98F0AFD-FEE6-443D-853C-DD8261A3B524}"/>
     <hyperlink ref="AC59" r:id="rId33" xr:uid="{A4613889-97D6-44B1-8EB3-E45E568562FF}"/>
+    <hyperlink ref="AC19" r:id="rId34" xr:uid="{0BE8AE82-9D3B-4B07-BDDB-C9896D570CF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>